<commit_message>
Merged Employees.xlsx into Cards.xlsx
</commit_message>
<xml_diff>
--- a/Cards.xlsx
+++ b/Cards.xlsx
@@ -9,12 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
     <sheet name="Bad Ideas" sheetId="2" r:id="rId2"/>
     <sheet name="Special Cards" sheetId="3" r:id="rId3"/>
+    <sheet name="Employees" sheetId="5" r:id="rId4"/>
+    <sheet name="Tally of Cards" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="109">
   <si>
     <t>Burn Rate Card Set</t>
   </si>
@@ -185,6 +187,174 @@
   </si>
   <si>
     <t>Opponent must pay double his or her burn rate next turn</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Regular Cards</t>
+  </si>
+  <si>
+    <t>Bad Ideas</t>
+  </si>
+  <si>
+    <t>Special Cards</t>
+  </si>
+  <si>
+    <t>Employees</t>
+  </si>
+  <si>
+    <t>Conclusion</t>
+  </si>
+  <si>
+    <t>My physical card set is complete</t>
+  </si>
+  <si>
+    <t>Contractor Cards (physical only)</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>Burn</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>Grant Stone</t>
+  </si>
+  <si>
+    <t>Manager</t>
+  </si>
+  <si>
+    <t>Andrew Chung</t>
+  </si>
+  <si>
+    <t>Brad Duke</t>
+  </si>
+  <si>
+    <t>VP</t>
+  </si>
+  <si>
+    <t>Martha Thule</t>
+  </si>
+  <si>
+    <t>Vern Slick</t>
+  </si>
+  <si>
+    <t>Charles Jackson</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>Brenda Swift</t>
+  </si>
+  <si>
+    <t>Georgia Gordon</t>
+  </si>
+  <si>
+    <t>Joel Jones</t>
+  </si>
+  <si>
+    <t>Barbara McNerny</t>
+  </si>
+  <si>
+    <t>Lacy Labonte</t>
+  </si>
+  <si>
+    <t>James Feasel</t>
+  </si>
+  <si>
+    <t>Martin Able</t>
+  </si>
+  <si>
+    <t>Chuck DeGaul</t>
+  </si>
+  <si>
+    <t>Finance</t>
+  </si>
+  <si>
+    <t>Ben Zhao</t>
+  </si>
+  <si>
+    <t>Sam Winters</t>
+  </si>
+  <si>
+    <t>Shannon Tyrell</t>
+  </si>
+  <si>
+    <t>Mary DeLany</t>
+  </si>
+  <si>
+    <t>Annette Chung</t>
+  </si>
+  <si>
+    <t>Hans Welch</t>
+  </si>
+  <si>
+    <t>Michael DeBeers</t>
+  </si>
+  <si>
+    <t>Development</t>
+  </si>
+  <si>
+    <t>Bob Headstein</t>
+  </si>
+  <si>
+    <t>Sally Hartwell</t>
+  </si>
+  <si>
+    <t>Niles Wheatly</t>
+  </si>
+  <si>
+    <t>Lawrence Smythe</t>
+  </si>
+  <si>
+    <t>Carrie Becker</t>
+  </si>
+  <si>
+    <t>Lance Slocum</t>
+  </si>
+  <si>
+    <t>Casey Close</t>
+  </si>
+  <si>
+    <t>Engineer</t>
+  </si>
+  <si>
+    <t>Tony Fuji</t>
+  </si>
+  <si>
+    <t>Harry Chin</t>
+  </si>
+  <si>
+    <t>Smedley Wilson</t>
+  </si>
+  <si>
+    <t>Bert Windage</t>
+  </si>
+  <si>
+    <t>Ed Syljik</t>
+  </si>
+  <si>
+    <t>Morton Baker</t>
+  </si>
+  <si>
+    <t>Gary Nasser</t>
+  </si>
+  <si>
+    <t>Carl Versace</t>
+  </si>
+  <si>
+    <t>Julie Malone</t>
+  </si>
+  <si>
+    <t>Contractors</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -504,8 +674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:C6"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -866,7 +1036,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="A22" sqref="A2:A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1246,4 +1416,660 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B18" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>83</v>
+      </c>
+      <c r="C19" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+      <c r="E20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>87</v>
+      </c>
+      <c r="C23" t="s">
+        <v>65</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>88</v>
+      </c>
+      <c r="C24" t="s">
+        <v>68</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+      <c r="E24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>89</v>
+      </c>
+      <c r="B26" t="s">
+        <v>90</v>
+      </c>
+      <c r="C26" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>91</v>
+      </c>
+      <c r="C27" t="s">
+        <v>68</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+      <c r="E27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>92</v>
+      </c>
+      <c r="C28" t="s">
+        <v>68</v>
+      </c>
+      <c r="D28">
+        <v>3</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>93</v>
+      </c>
+      <c r="C29" t="s">
+        <v>65</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C30" t="s">
+        <v>65</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>95</v>
+      </c>
+      <c r="C31" t="s">
+        <v>65</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>96</v>
+      </c>
+      <c r="C32" t="s">
+        <v>97</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>98</v>
+      </c>
+      <c r="C33" t="s">
+        <v>97</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>99</v>
+      </c>
+      <c r="C34" t="s">
+        <v>97</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>100</v>
+      </c>
+      <c r="C35" t="s">
+        <v>97</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>101</v>
+      </c>
+      <c r="C36" t="s">
+        <v>97</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>102</v>
+      </c>
+      <c r="C37" t="s">
+        <v>97</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>103</v>
+      </c>
+      <c r="C38" t="s">
+        <v>97</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>104</v>
+      </c>
+      <c r="C39" t="s">
+        <v>97</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>105</v>
+      </c>
+      <c r="C40" t="s">
+        <v>97</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>106</v>
+      </c>
+      <c r="C41" t="s">
+        <v>97</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>107</v>
+      </c>
+      <c r="B43" t="s">
+        <v>108</v>
+      </c>
+      <c r="C43" t="s">
+        <v>108</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8">
+        <f>SUM(B1:B6)</f>
+        <v>154</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>